<commit_message>
stand bijgewerkt tot 28-10-2016
</commit_message>
<xml_diff>
--- a/data/Austerlitz_seizoen_2016-2017.xlsx
+++ b/data/Austerlitz_seizoen_2016-2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2016-09-02" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,8 @@
     <sheet name="2016-09-30" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2016-10-07" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="2016-10-14" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="2016-10-21" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="2016-10-28" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="42">
   <si>
     <t xml:space="preserve">Baan</t>
   </si>
@@ -260,7 +262,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,7 +1019,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2034,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +2997,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,7 +3997,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,6 +4913,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5700,8 +5705,1005 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5749,87 +6751,90 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -5838,27 +6843,30 @@
         <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2</v>
@@ -5869,22 +6877,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5892,13 +6900,813 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L45"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2</v>
@@ -5909,42 +7717,45 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5955,30 +7766,33 @@
         <v>4</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
@@ -5989,85 +7803,82 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6078,10 +7889,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -6092,16 +7903,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>2</v>
@@ -6112,56 +7923,59 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E20" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>40</v>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>2</v>
@@ -6172,168 +7986,168 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H30" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6344,7 +8158,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>20</v>
@@ -6355,39 +8169,42 @@
       <c r="F31" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="L31" s="0" t="n">
+        <v>143</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
@@ -6401,39 +8218,42 @@
         <v>4</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6441,36 +8261,36 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="E37" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>2</v>
@@ -6484,10 +8304,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>2</v>
@@ -6504,33 +8324,33 @@
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>2</v>
@@ -6538,65 +8358,68 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6607,10 +8430,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
@@ -6621,61 +8444,21 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="0" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stand 11-11 + changes printing
</commit_message>
<xml_diff>
--- a/data/Austerlitz_seizoen_2016-2017.xlsx
+++ b/data/Austerlitz_seizoen_2016-2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="2016-09-02" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="2016-10-21" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="2016-10-28" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="2016-11-04" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="2016-11-11" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="44">
   <si>
     <t xml:space="preserve">Baan</t>
   </si>
@@ -159,6 +160,9 @@
   <si>
     <t xml:space="preserve">Kim</t>
   </si>
+  <si>
+    <t xml:space="preserve">nye</t>
+  </si>
 </sst>
 </file>
 
@@ -266,7 +270,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,13 +1021,896 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L43"/>
+  <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,128 +1953,125 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>105</v>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2</v>
@@ -1198,22 +2082,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,16 +2108,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,16 +2128,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="E10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,33 +2148,33 @@
         <v>4</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
@@ -1298,22 +2182,22 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,13 +2205,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0</v>
@@ -1338,16 +2222,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
@@ -1358,42 +2242,42 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,16 +2288,16 @@
         <v>3</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="E18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,56 +2308,59 @@
         <v>3</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,13 +2368,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
@@ -1498,44 +2385,44 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1547,27 +2434,27 @@
         <v>2</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>13</v>
@@ -1587,16 +2474,16 @@
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E27" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,16 +2494,16 @@
         <v>2</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>15</v>
@@ -1638,9 +2525,6 @@
       <c r="F29" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1650,13 +2534,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>2</v>
@@ -1670,15 +2554,18 @@
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1687,96 +2574,93 @@
         <v>2</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>0</v>
@@ -1787,59 +2671,59 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>2</v>
@@ -1847,16 +2731,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1</v>
@@ -1867,22 +2751,62 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>2</v>
+      <c r="D42" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1909,7 +2833,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +3848,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,6 +4810,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4884,7 +5811,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5800,9 +6727,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6597,6 +7521,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7592,7 +8519,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8398,7 +9325,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>